<commit_message>
Página de estadísticas y equipos actualizados
</commit_message>
<xml_diff>
--- a/excels/equipos_actas.xlsx
+++ b/excels/equipos_actas.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unexes-my.sharepoint.com/personal/rvicenteg_alumnos_unex_es/Documents/UNIVERSIDAD/.resto/liga_futbol/Liga-de-Futbol-CUMe/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_E7ED0E6FA2C5B44F6654A01E966996A7AB9E760C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FDD0597A-DA36-4B98-B6A3-C5778B22181F}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_E7ED0E6FA2C5B44F6654A01E966996A7AB9E760C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60553BF1-720B-40BC-A455-B555CBBF336C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CUM UNITED" sheetId="1" r:id="rId1"/>
-    <sheet name="RAYO MARIGUANO" sheetId="3" r:id="rId2"/>
+    <sheet name="ATLÉTICO MORANTE" sheetId="5" r:id="rId1"/>
+    <sheet name="CUM UNITED" sheetId="1" r:id="rId2"/>
+    <sheet name="CERVEZA FC" sheetId="4" r:id="rId3"/>
+    <sheet name="RAYO MARIGUANO" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>CUM UNITED</t>
   </si>
@@ -129,6 +131,81 @@
   </si>
   <si>
     <t>images/Escudos/CUM UNITED.png</t>
+  </si>
+  <si>
+    <t>images/Escudos/CERVEZA.png</t>
+  </si>
+  <si>
+    <t>CERVEZA FC</t>
+  </si>
+  <si>
+    <t>Iván Rodríguez Sepúlveda</t>
+  </si>
+  <si>
+    <t>Isidro Capitán Torres</t>
+  </si>
+  <si>
+    <t>David Gómez Ruiz</t>
+  </si>
+  <si>
+    <t>Carlos Borja Vaquero</t>
+  </si>
+  <si>
+    <t>Antonio Carrasco Marchante</t>
+  </si>
+  <si>
+    <t>Javier Conejero Rodríguez</t>
+  </si>
+  <si>
+    <t>Antonio González Reyes</t>
+  </si>
+  <si>
+    <t>Rubén Garrido Calderón</t>
+  </si>
+  <si>
+    <t>Álvaro Clavero Irastorza</t>
+  </si>
+  <si>
+    <t>Izan Campanón López</t>
+  </si>
+  <si>
+    <t>images/Escudos/MORANTE.png</t>
+  </si>
+  <si>
+    <t>ATLÉTICO MORANTE</t>
+  </si>
+  <si>
+    <t>Manuel Mestre Martín</t>
+  </si>
+  <si>
+    <t>Carlos Fuentes García</t>
+  </si>
+  <si>
+    <t>Daniel Gallego Tabla</t>
+  </si>
+  <si>
+    <t>Javier Fernández Delgado</t>
+  </si>
+  <si>
+    <t>Álvaro Fuentes Delgado</t>
+  </si>
+  <si>
+    <t>Gonzalo García Díaz</t>
+  </si>
+  <si>
+    <t>Vicente Collado Jurado</t>
+  </si>
+  <si>
+    <t>Luis Miguel Lavado Gómez</t>
+  </si>
+  <si>
+    <t>Javier Herrero Ruiz</t>
+  </si>
+  <si>
+    <t>Pedro José Padilla Ramírez</t>
+  </si>
+  <si>
+    <t>images/jugadores/vini.png</t>
   </si>
 </sst>
 </file>
@@ -161,9 +238,8 @@
       <name val="Montserrat"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <scheme val="minor"/>
@@ -212,7 +288,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -780,13 +856,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51A4A07-EF69-4C9B-A54A-8C425DB94255}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="45.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -941,14 +1176,173 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9033F9-C056-414C-AC92-C8D8EFAF05EB}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="45.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED22726-50E8-443A-8D68-C529969A71D9}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -973,41 +1367,61 @@
       <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="C7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1015,17 +1429,26 @@
       <c r="B12" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Actualización mitad de liga.
</commit_message>
<xml_diff>
--- a/excels/equipos_actas.xlsx
+++ b/excels/equipos_actas.xlsx
@@ -1,29 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unexes-my.sharepoint.com/personal/rvicenteg_alumnos_unex_es/Documents/UNIVERSIDAD/.resto/liga_futbol/Liga-de-Futbol-CUMe/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_E7ED0E6FA2C5B44F6654A01E966996A7AB9E760C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60553BF1-720B-40BC-A455-B555CBBF336C}"/>
+  <xr:revisionPtr revIDLastSave="280" documentId="11_E7ED0E6FA2C5B44F6654A01E966996A7AB9E760C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A35FBA83-7201-4A2F-A842-9DBCA95505F5}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="0" windowWidth="19200" windowHeight="9970" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ATLÉTICO MORANTE" sheetId="5" r:id="rId1"/>
-    <sheet name="CUM UNITED" sheetId="1" r:id="rId2"/>
-    <sheet name="CERVEZA FC" sheetId="4" r:id="rId3"/>
-    <sheet name="RAYO MARIGUANO" sheetId="3" r:id="rId4"/>
+    <sheet name="CUM UNITED" sheetId="1" r:id="rId1"/>
+    <sheet name="RAYO MARIGUANO" sheetId="3" r:id="rId2"/>
+    <sheet name="ATLÉTICO MORANTE" sheetId="5" r:id="rId3"/>
+    <sheet name="ASTON BIRRA" sheetId="4" r:id="rId4"/>
+    <sheet name="I.E. SALA" sheetId="6" r:id="rId5"/>
+    <sheet name="CUM CITY" sheetId="7" r:id="rId6"/>
+    <sheet name="UNIÓN DEPORTIVA PORRETA" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="154">
   <si>
     <t>CUM UNITED</t>
   </si>
@@ -112,9 +115,6 @@
     <t>images/jugadores/cumUnited/juan.png</t>
   </si>
   <si>
-    <t>images/jugadores/cumUnited/vini.png</t>
-  </si>
-  <si>
     <t>images/jugadores/cumUnited/daniel.png</t>
   </si>
   <si>
@@ -127,18 +127,9 @@
     <t>images/jugadores/cumUnited/juanki.png</t>
   </si>
   <si>
-    <t>images/Escudos/RAYO.png</t>
-  </si>
-  <si>
     <t>images/Escudos/CUM UNITED.png</t>
   </si>
   <si>
-    <t>images/Escudos/CERVEZA.png</t>
-  </si>
-  <si>
-    <t>CERVEZA FC</t>
-  </si>
-  <si>
     <t>Iván Rodríguez Sepúlveda</t>
   </si>
   <si>
@@ -169,9 +160,6 @@
     <t>Izan Campanón López</t>
   </si>
   <si>
-    <t>images/Escudos/MORANTE.png</t>
-  </si>
-  <si>
     <t>ATLÉTICO MORANTE</t>
   </si>
   <si>
@@ -205,14 +193,308 @@
     <t>Pedro José Padilla Ramírez</t>
   </si>
   <si>
-    <t>images/jugadores/vini.png</t>
+    <t>I.E. SALA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fabio Sánchez Jiménez </t>
+  </si>
+  <si>
+    <t>Ángel Carapeto Mauriz</t>
+  </si>
+  <si>
+    <t>Marcos Ocaña Santamaría</t>
+  </si>
+  <si>
+    <t>Juan Luís Rodríguez Hernández</t>
+  </si>
+  <si>
+    <t>David Fernández Rubio</t>
+  </si>
+  <si>
+    <t>Víctor Álvarez Ordoñez</t>
+  </si>
+  <si>
+    <t>images/Escudos/I.E. SALA.png</t>
+  </si>
+  <si>
+    <t>Carlos Frejido Mínguez</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/carlos.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/alejandro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/david.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/francisco.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/fernando.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/alvaro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/gonzalo.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/josemaria.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/francisco2.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/juan.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/rayo/lucia.jpg</t>
+  </si>
+  <si>
+    <t>CUM CITY</t>
+  </si>
+  <si>
+    <t>Carlos Zambrano Ruiz</t>
+  </si>
+  <si>
+    <t>images/Escudos/CUM CITY.png</t>
+  </si>
+  <si>
+    <t>23. David Cáceres Valle</t>
+  </si>
+  <si>
+    <t>8. Andrés Pajuelo Sánchez</t>
+  </si>
+  <si>
+    <t>67. Justo Manuel Sánchez Triguero</t>
+  </si>
+  <si>
+    <t>37. Alberto Durán López</t>
+  </si>
+  <si>
+    <t>45. Juan Pietro Da Silva Martins</t>
+  </si>
+  <si>
+    <t>10. Juan Luís Fernández Gómez de Villar</t>
+  </si>
+  <si>
+    <t>4. Luís Miguel Márquez Parrado</t>
+  </si>
+  <si>
+    <t>3. Ciro Benjamín Castañeda Flores</t>
+  </si>
+  <si>
+    <t>images/jugadores/blank.png</t>
+  </si>
+  <si>
+    <t>ASTON BIRRA</t>
+  </si>
+  <si>
+    <t>Víctor Pérez Castro</t>
+  </si>
+  <si>
+    <t>Pablo Mimbrero González</t>
+  </si>
+  <si>
+    <t>images/Escudos/UNIÓN DEPORTIVA PORRETA.png</t>
+  </si>
+  <si>
+    <t>UNIÓN DEPORTIVA PORRETA</t>
+  </si>
+  <si>
+    <t>José María Cabezas Rua</t>
+  </si>
+  <si>
+    <t>Alberto Salazar Muñoz</t>
+  </si>
+  <si>
+    <t>Hugo Segovia Espinosa</t>
+  </si>
+  <si>
+    <t>Asier Mariño de Prado</t>
+  </si>
+  <si>
+    <t>Víctor Santamaría</t>
+  </si>
+  <si>
+    <t>Alejandro Cancho Rodríguez</t>
+  </si>
+  <si>
+    <t>Ángel Moreno Rojas</t>
+  </si>
+  <si>
+    <t>Francisco José Carretero Pablos</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/ciro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/manuel.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/carlos.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/daniel.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/javier.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/alvaro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/gonzalo.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/vicente.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/luismi.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/morante/pedro.jpg</t>
+  </si>
+  <si>
+    <t>images/Escudos/ASTON BIRRA.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/ivan.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/isidro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/david.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/carlos.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/antonio.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/ruben.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/alvaro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/izan.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/victor.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/pablo.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/javi.jpg</t>
+  </si>
+  <si>
+    <t>images/Escudos/RAYO MARIGUANO.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/marcos.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/victor.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/fabio.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/angel.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/juanluis.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/david.png</t>
+  </si>
+  <si>
+    <t>Aarón Molina Cuadrado</t>
+  </si>
+  <si>
+    <t>images/jugadores/iesala/aaron.png</t>
+  </si>
+  <si>
+    <t>Álvaro Gobernado</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/josemaria.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/alberto.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/hugo.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/asier.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/angel.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/victor.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/aston/antonio2.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/alex.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/alvaro.jpg</t>
+  </si>
+  <si>
+    <t>Francisco Javier Castro García</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/fcojavier.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/udp/fran.jpg</t>
+  </si>
+  <si>
+    <t>images/Escudos/ATLÉTICO MORANTE.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/carlos.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/david.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/andres.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/justo.png</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/alberto.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/pietro.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/juanlu.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumCity/luismi.jpg</t>
+  </si>
+  <si>
+    <t>images/jugadores/cumUnited/mario.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -244,6 +526,19 @@
       <family val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -271,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -289,6 +584,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -856,170 +1157,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51A4A07-EF69-4C9B-A54A-8C425DB94255}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:C24"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="25.296875" customWidth="1"/>
-    <col min="2" max="2" width="45.296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1032,10 +1176,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1101,7 +1245,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1110,7 +1254,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1119,7 +1263,7 @@
         <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1128,7 +1272,7 @@
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1137,34 +1281,58 @@
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C23" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
     </row>
   </sheetData>
@@ -1176,15 +1344,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9033F9-C056-414C-AC92-C8D8EFAF05EB}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED22726-50E8-443A-8D68-C529969A71D9}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1195,134 +1363,342 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+        <v>122</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>37</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
+        <v>13</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
-        <v>60</v>
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s">
-        <v>60</v>
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
+        <v>16</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
+        <v>17</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
+        <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
+        <v>19</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
+        <v>21</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+      <c r="C23" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51A4A07-EF69-4C9B-A54A-8C425DB94255}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="45.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
         <v>47</v>
       </c>
+      <c r="C7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
+      <c r="C15" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C22" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
     </row>
   </sheetData>
@@ -1334,14 +1710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ED22726-50E8-443A-8D68-C529969A71D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9033F9-C056-414C-AC92-C8D8EFAF05EB}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1352,134 +1728,680 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+        <v>110</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
+        <v>40</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5226715A-2177-4D28-B541-4937F00AB848}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="45.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
         <v>60</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="7" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="2"/>
+      <c r="C15" s="7" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE27DBB-DCED-47EC-AEC6-077941F9C77A}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="45.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="13" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{843BD545-8DAC-41FB-B91C-2570462EFA2A}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.296875" customWidth="1"/>
+    <col min="2" max="2" width="45.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" s="2"/>
+      <c r="C16" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" s="2"/>
+      <c r="C17" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" s="2"/>
+      <c r="C18" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" s="2"/>
+      <c r="C19" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+      <c r="C20" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+      <c r="C21" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+      <c r="C22" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementado Supabase + Actas dinámicas
</commit_message>
<xml_diff>
--- a/excels/equipos_actas.xlsx
+++ b/excels/equipos_actas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unexes-my.sharepoint.com/personal/rvicenteg_alumnos_unex_es/Documents/UNIVERSIDAD/.resto/liga_futbol/Liga-de-Futbol-CUMe/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Uni\OneDrive - Universidad de Extremadura\UNIVERSIDAD\.resto\liga_futbol\Liga-de-Futbol-CUMe\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="11_E7ED0E6FA2C5B44F6654A01E966996A7AB9E760C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A35FBA83-7201-4A2F-A842-9DBCA95505F5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14EFE1E-B0CD-4F09-84B0-E730D62AA8BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CUM UNITED" sheetId="1" r:id="rId1"/>
@@ -325,9 +325,6 @@
     <t>Ángel Moreno Rojas</t>
   </si>
   <si>
-    <t>Francisco José Carretero Pablos</t>
-  </si>
-  <si>
     <t>images/jugadores/cumCity/ciro.jpg</t>
   </si>
   <si>
@@ -451,9 +448,6 @@
     <t>images/jugadores/udp/alvaro.jpg</t>
   </si>
   <si>
-    <t>Francisco Javier Castro García</t>
-  </si>
-  <si>
     <t>images/jugadores/udp/fcojavier.jpg</t>
   </si>
   <si>
@@ -488,6 +482,12 @@
   </si>
   <si>
     <t>images/jugadores/cumUnited/mario.jpg</t>
+  </si>
+  <si>
+    <t>Francisco Javier Carretero García</t>
+  </si>
+  <si>
+    <t>Francisco José Castro Pablos</t>
   </si>
 </sst>
 </file>
@@ -956,10 +956,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -1163,7 +1159,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1245,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1363,7 +1359,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1547,7 +1543,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1563,7 +1559,7 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1572,7 +1568,7 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1581,7 +1577,7 @@
         <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1590,7 +1586,7 @@
         <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1599,7 +1595,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1608,7 +1604,7 @@
         <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1616,7 +1612,7 @@
         <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,7 +1621,7 @@
         <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1634,7 +1630,7 @@
         <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1643,7 +1639,7 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1728,7 +1724,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1744,7 +1740,7 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1753,7 +1749,7 @@
         <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1762,7 +1758,7 @@
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1771,7 +1767,7 @@
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1780,7 +1776,7 @@
         <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1789,7 +1785,7 @@
         <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1797,7 +1793,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1806,7 +1802,7 @@
         <v>41</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1815,7 +1811,7 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1824,7 +1820,7 @@
         <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1833,7 +1829,7 @@
         <v>88</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1841,7 +1837,7 @@
         <v>89</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
@@ -1929,7 +1925,7 @@
         <v>56</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1938,7 +1934,7 @@
         <v>57</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1947,7 +1943,7 @@
         <v>58</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1956,7 +1952,7 @@
         <v>59</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1965,7 +1961,7 @@
         <v>60</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1974,15 +1970,15 @@
         <v>61</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2092,7 +2088,7 @@
         <v>76</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2101,7 +2097,7 @@
         <v>78</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2110,7 +2106,7 @@
         <v>79</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2119,7 +2115,7 @@
         <v>80</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2128,7 +2124,7 @@
         <v>81</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2137,7 +2133,7 @@
         <v>82</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2145,7 +2141,7 @@
         <v>83</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2154,7 +2150,7 @@
         <v>84</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2163,7 +2159,7 @@
         <v>85</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2238,8 +2234,8 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2263,10 +2259,10 @@
     <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16.5" x14ac:dyDescent="0.3">
@@ -2275,7 +2271,7 @@
         <v>92</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2284,7 +2280,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2293,7 +2289,7 @@
         <v>94</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2302,7 +2298,7 @@
         <v>95</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2311,7 +2307,7 @@
         <v>96</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2319,7 +2315,7 @@
         <v>97</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2328,25 +2324,25 @@
         <v>98</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="B13" s="2" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>